<commit_message>
added header row of names
</commit_message>
<xml_diff>
--- a/ch03/geodata/highest-mountains-europe.xlsx
+++ b/ch03/geodata/highest-mountains-europe.xlsx
@@ -15,7 +15,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>GeoNameId</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
   <si>
     <t>Mount Ararat</t>
   </si>
@@ -78,6 +96,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,7 +161,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,13 +180,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -178,162 +197,182 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>325164</v>
+      <c r="A1" s="0" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>39.70224</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>44.298</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5165</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>3181986</v>
+        <v>325164</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45.833</v>
+        <v>39.70224</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>6.864</v>
+        <v>44.298</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>4810</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2641744</v>
+        <v>3181986</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>56.79656</v>
+        <v>45.833</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>-5.00393</v>
+        <v>6.864</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>1344</v>
+        <v>4810</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>734890</v>
+        <v>2641744</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>40.08175</v>
+        <v>56.79656</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>22.34954</v>
+        <v>-5.00393</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>2917</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>2411583</v>
+        <v>734890</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>36.14363</v>
+        <v>40.08175</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>-5.34296</v>
+        <v>22.34954</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>426</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>3188835</v>
+        <v>2411583</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>46.37823</v>
+        <v>36.14363</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>13.83671</v>
+        <v>-5.34296</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>2864</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>2760454</v>
+        <v>3188835</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>47.42118</v>
+        <v>46.37823</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>10.98635</v>
+        <v>13.83671</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>2962</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
+        <v>2760454</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>47.42118</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>10.98635</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2962</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>3085294</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="n">
+      <c r="B9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>50.73609</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E9" s="1" t="n">
         <v>15.73979</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>1602</v>
       </c>
     </row>

</xml_diff>